<commit_message>
Added a few more entires
</commit_message>
<xml_diff>
--- a/Doctor Search.xlsx
+++ b/Doctor Search.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmalee/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LilyHe/Downloads/CS2a final_project/final_project-master 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15320" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="9240" yWindow="780" windowWidth="16360" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>City</t>
   </si>
@@ -93,6 +93,66 @@
   </si>
   <si>
     <t>Boston Children's Hospital</t>
+  </si>
+  <si>
+    <t>Denise</t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>02451</t>
+  </si>
+  <si>
+    <t>Donald</t>
+  </si>
+  <si>
+    <t>Bae</t>
+  </si>
+  <si>
+    <t>Mass General Hospital</t>
+  </si>
+  <si>
+    <t>02114</t>
+  </si>
+  <si>
+    <t>Vicki</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Raff</t>
+  </si>
+  <si>
+    <t>Lynn</t>
+  </si>
+  <si>
+    <t>Wachs</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Sabatini</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Faquin</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Bauer</t>
   </si>
 </sst>
 </file>
@@ -108,14 +168,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF374249"/>
-      <name val="Inherit"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Museo_sans100"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Times Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,9 +201,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,186 +484,319 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>7814874340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>7814874340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>7814874340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>7814874340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7814874340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2">
+      <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2">
+        <v>7818942996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2">
+        <v>6173555226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2">
+        <v>6173556021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6173556021</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="2">
+        <v>6177249197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="2">
+        <v>6177262914</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2">
         <v>7814874340</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>7814874340</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>7814874340</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>7814874340</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>7814874340</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="4">
-        <v>7818942996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="D8" s="3"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="E15" s="1"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6177268868</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="2">
+        <v>6175733957</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added doc_search.py (very basic filtering for now)
</commit_message>
<xml_diff>
--- a/Doctor Search.xlsx
+++ b/Doctor Search.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LilyHe/Downloads/CS2a final_project/final_project-master 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LilyHe/Downloads/CS2a final_project/final_project-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="780" windowWidth="16360" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
     <t>Zip</t>
   </si>
   <si>
-    <t xml:space="preserve">Hospital </t>
-  </si>
-  <si>
     <t>Phone Number</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>Bauer</t>
+  </si>
+  <si>
+    <t>Hospital</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,10 +498,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -510,27 +510,27 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2">
         <v>7814874340</v>
@@ -538,19 +538,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
         <v>7814874340</v>
@@ -558,19 +558,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2">
         <v>7814874340</v>
@@ -578,19 +578,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
         <v>7814874340</v>
@@ -598,19 +598,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2">
         <v>7814874340</v>
@@ -618,19 +618,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="F7" s="2">
         <v>7818942996</v>
@@ -638,19 +638,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="2">
         <v>6173555226</v>
@@ -658,19 +658,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2">
         <v>6173556021</v>
@@ -678,19 +678,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1">
         <v>6173556021</v>
@@ -698,19 +698,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="2">
         <v>6177249197</v>
@@ -718,19 +718,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="2">
         <v>6177262914</v>
@@ -738,19 +738,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="2">
         <v>7814874340</v>
@@ -758,19 +758,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="2">
         <v>6177268868</v>
@@ -778,19 +778,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="2">
         <v>6175733957</v>

</xml_diff>